<commit_message>
refs #3.1 Data update
</commit_message>
<xml_diff>
--- a/SSWebScraper/SSWebScraper/Data/SeedData/DataSheets/BodyTypeLanguage.xlsx
+++ b/SSWebScraper/SSWebScraper/Data/SeedData/DataSheets/BodyTypeLanguage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T480\Desktop\MarketWatch\SSWebScraper\SSWebScraper\Data\SeedData\DataSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44895AA4-F0C3-419D-BB63-A09D869B909B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CAAE3A-04AE-4344-8FFA-CA1884A3D027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-5340" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>BodyTypeId</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>DisplayOrder</t>
   </si>
   <si>
     <t>-</t>
@@ -384,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C11"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -398,7 +395,7 @@
     <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,25 +405,19 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -434,13 +425,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -448,13 +436,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -462,13 +447,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -476,13 +458,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -490,13 +469,10 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -504,13 +480,10 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -518,13 +491,10 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -532,13 +502,10 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -546,10 +513,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>